<commit_message>
ADD changes in main with changes in the principal document word "plantilla" and resolve the problemes on the principals function
</commit_message>
<xml_diff>
--- a/detallesBasedatosPrueba.xlsx
+++ b/detallesBasedatosPrueba.xlsx
@@ -9,19 +9,27 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -45,17 +53,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +462,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -468,149 +477,156 @@
     <col width="29.140625" customWidth="1" min="5" max="5"/>
     <col width="17" customWidth="1" min="6" max="6"/>
     <col width="31.85546875" customWidth="1" min="8" max="8"/>
+    <col width="34.28515625" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Titulo de Credito </t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">RUC </t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">ID Number </t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CONCEPTO </t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">VALOR CAPITAL </t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>VALOS  30%</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concepto </t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Valor Capital</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Valor 30%</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Lawyer</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Judge</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n"/>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="n"/>
-      <c r="H6" s="2" t="n"/>
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="n"/>
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" s="2" t="n"/>
-      <c r="F8" s="2" t="n"/>
-      <c r="G8" s="2" t="n"/>
-      <c r="H8" s="2" t="n"/>
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="3" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="3" t="n"/>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" s="2" t="n"/>
-      <c r="G10" s="2" t="n"/>
-      <c r="H10" s="2" t="n"/>
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="4" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
-      <c r="F11" s="2" t="n"/>
-      <c r="G11" s="2" t="n"/>
-      <c r="H11" s="2" t="n"/>
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -958,6 +974,11 @@
           <t>Dr. Christian Santiago Izurieta Cruz</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Ing. AAAA</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -985,8 +1006,10 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>100.25</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>100.25</t>
+        </is>
       </c>
       <c r="G21" t="n">
         <v>100</v>
@@ -999,6 +1022,11 @@
           <t>Dr. Christian Santiago Izurieta Cruz</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Ing. AAAA</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1026,18 +1054,25 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>152.23</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>152.23</t>
+        </is>
       </c>
       <c r="G22" t="n">
         <v>204.26</v>
       </c>
       <c r="H22" t="n">
-        <v>265.538</v>
+        <v>265.54</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
         </is>
       </c>
     </row>
@@ -1067,18 +1102,25 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>98.56</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>98.56</t>
+        </is>
       </c>
       <c r="G23" t="n">
         <v>150.47</v>
       </c>
       <c r="H23" t="n">
-        <v>195.611</v>
+        <v>195.61</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
           <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
         </is>
       </c>
     </row>
@@ -1108,18 +1150,25 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>78.54000000000001</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>78.54</t>
+        </is>
       </c>
       <c r="G24" t="n">
         <v>123.25</v>
       </c>
       <c r="H24" t="n">
-        <v>160.225</v>
+        <v>160.22</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
         </is>
       </c>
     </row>
@@ -1149,8 +1198,10 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>55.85</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>55.85</t>
+        </is>
       </c>
       <c r="G25" t="n">
         <v>89.90000000000001</v>
@@ -1163,6 +1214,11 @@
           <t>Dr. Christian Santiago Izurieta Cruz</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1190,18 +1246,167 @@
           <t>PLANTILLA DE APORTES</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>66.58</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>66.58</t>
+        </is>
       </c>
       <c r="G26" t="n">
         <v>94.84999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>123.305</v>
+        <v>123.3</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>457878</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>456789123</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>PLANTILLA DE APORTES</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>124.25</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>453.26</v>
+      </c>
+      <c r="H27" t="n">
+        <v>589.24</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Ing. AAAA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Peter Patricio Tene Ojeda</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>174582556</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>174582556001</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>PLANTILLA DE APORTES</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>45.85</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>245.58</v>
+      </c>
+      <c r="H28" t="n">
+        <v>319.25</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Peter Patricio Tene Ojeda</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>174582556</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>174582556001</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>PLANTILLA DE APORTES</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>12.25</v>
+      </c>
+      <c r="G29" t="n">
+        <v>245.58</v>
+      </c>
+      <c r="H29" t="n">
+        <v>319.254</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Lic. Alexander Javier Miranda Granero</t>
         </is>
       </c>
     </row>

</xml_diff>